<commit_message>
refit distributions to updated SPADE output
</commit_message>
<xml_diff>
--- a/data/SPADE_nutrient_key.xlsx
+++ b/data/SPADE_nutrient_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/subnational_nutrient_distributions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A02626-1F31-3042-916A-0AFE488D66CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C688CC-F8DE-B24B-A68E-E1CD63D00FC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="1960" windowWidth="30600" windowHeight="21460" xr2:uid="{A28501FA-7E3C-C044-BF79-67C6D0402D20}"/>
+    <workbookView xWindow="14320" yWindow="500" windowWidth="30600" windowHeight="21460" xr2:uid="{A28501FA-7E3C-C044-BF79-67C6D0402D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="78">
   <si>
     <t>mg</t>
   </si>
@@ -232,6 +232,33 @@
   </si>
   <si>
     <t>Lutein and zeaxanthin</t>
+  </si>
+  <si>
+    <t>Biotin</t>
+  </si>
+  <si>
+    <t>Vitamin B7</t>
+  </si>
+  <si>
+    <t>Caffeine</t>
+  </si>
+  <si>
+    <t>Chromium</t>
+  </si>
+  <si>
+    <t>Vitamin B5</t>
+  </si>
+  <si>
+    <t>Pantothenic acid</t>
+  </si>
+  <si>
+    <t>Vitamin A (RE)</t>
+  </si>
+  <si>
+    <t>Cobalamin</t>
+  </si>
+  <si>
+    <t>Pyridoxine</t>
   </si>
 </sst>
 </file>
@@ -593,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CA9292-CB8C-B341-96A9-A1A7DC149A4D}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,72 +654,77 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -703,8 +735,9 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
@@ -717,8 +750,9 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
@@ -731,8 +765,9 @@
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
@@ -745,8 +780,9 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
@@ -759,8 +795,9 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
@@ -770,13 +807,14 @@
         <v>64</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -784,11 +822,12 @@
         <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
@@ -798,11 +837,12 @@
         <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
@@ -812,13 +852,14 @@
         <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -826,83 +867,89 @@
         <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -910,13 +957,14 @@
         <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -924,13 +972,14 @@
         <v>65</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -938,13 +987,14 @@
         <v>65</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,13 +1002,14 @@
         <v>65</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -966,13 +1017,14 @@
         <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,8 +1035,9 @@
         <v>21</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>0</v>
       </c>
@@ -997,167 +1050,176 @@
         <v>21</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" t="s">
-        <v>63</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1168,13 +1230,13 @@
         <v>44</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1185,10 +1247,10 @@
         <v>44</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>4</v>
@@ -1202,10 +1264,10 @@
         <v>44</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>0</v>
@@ -1219,10 +1281,10 @@
         <v>44</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>0</v>
@@ -1236,7 +1298,10 @@
         <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>4</v>
@@ -1250,7 +1315,10 @@
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>0</v>
@@ -1264,7 +1332,10 @@
         <v>44</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>0</v>
@@ -1278,8 +1349,9 @@
         <v>44</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
         <v>4</v>
       </c>
@@ -1292,8 +1364,9 @@
         <v>44</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
         <v>0</v>
       </c>
@@ -1306,16 +1379,97 @@
         <v>44</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E49">
-    <sortCondition ref="A2:A49"/>
-    <sortCondition ref="B2:B49"/>
+  <sortState ref="A2:E54">
+    <sortCondition ref="B2:B54"/>
+    <sortCondition ref="A2:A54"/>
+    <sortCondition ref="C2:C54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>